<commit_message>
Casos de prueba y videos
</commit_message>
<xml_diff>
--- a/Actividad 3 & 4/CasosDePrueba.xlsx
+++ b/Actividad 3 & 4/CasosDePrueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60ab0c85b300754c/Documentos/Ibero/6to/BDA/Actividades_BDA/Actividad 3 ^0 4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5DC877E6-5A82-4F39-80FD-4846329D3EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="8_{5DC877E6-5A82-4F39-80FD-4846329D3EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7DABDD0-126E-47F0-8C44-EF2312C1BDBF}"/>
   <bookViews>
-    <workbookView xWindow="2850" yWindow="3495" windowWidth="20430" windowHeight="11520" xr2:uid="{FA6954D8-D278-4FDC-A4AB-12ABCB0B670E}"/>
+    <workbookView xWindow="17340" yWindow="255" windowWidth="20430" windowHeight="11520" xr2:uid="{FA6954D8-D278-4FDC-A4AB-12ABCB0B670E}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Prueba" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>No.</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>Resultados Esperados</t>
-  </si>
-  <si>
-    <t>Pos Condición</t>
   </si>
   <si>
     <t>Estado</t>
@@ -93,12 +90,6 @@
 2. Registrar el tiempo de respuesta de cada solicitud</t>
   </si>
   <si>
-    <t>El tiempo en manejar las solicitudes debe ser menor a 2 segundos y no debe exceder los 10 segundos</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Alta</t>
   </si>
   <si>
@@ -121,15 +112,6 @@
 2. Registrar tiempos de respuesta</t>
   </si>
   <si>
-    <t>Las solicitudes deben ser manejadas en menos de un minto</t>
-  </si>
-  <si>
-    <t>Tiempo de respuesta</t>
-  </si>
-  <si>
-    <t>Aprobado</t>
-  </si>
-  <si>
     <t>Media</t>
   </si>
   <si>
@@ -145,6 +127,15 @@
   </si>
   <si>
     <t>Cada shard tiene al menos una réplica funcional</t>
+  </si>
+  <si>
+    <t>Las solicitudes deben ser manejadas en menos de un minuto</t>
+  </si>
+  <si>
+    <t>El tiempo en manejar las solicitudes debe ser menor a 2 segundos</t>
+  </si>
+  <si>
+    <t>Aprobado</t>
   </si>
 </sst>
 </file>
@@ -437,6 +428,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -736,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A988ED3-D3B7-4385-9824-5CE89AA3C35A}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="I5" sqref="A1:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,17 +746,16 @@
     <col min="5" max="5" width="26.140625" customWidth="1"/>
     <col min="6" max="6" width="29.85546875" customWidth="1"/>
     <col min="7" max="7" width="29.42578125" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>1</v>
@@ -781,139 +775,124 @@
       <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="8" t="s">
+      <c r="F3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="9" t="s">
+    </row>
+    <row r="5" spans="1:9" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>3</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>4</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="15" t="s">
+      <c r="H5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
-        <v>5</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>20</v>
+      <c r="I5" s="14" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>